<commit_message>
Finishing up Documentation for Week 10 Turn In
</commit_message>
<xml_diff>
--- a/Week 10 Gantt Chart.xlsx
+++ b/Week 10 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{C89E6D09-F279-40DD-B44D-6FB2B39E463D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17B392B7-A1C1-4F84-9C3C-61E43E3984DC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABBDB44-0EAF-4315-AA4D-46C41F80F4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>Project Start:</t>
   </si>
@@ -1470,11 +1470,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BL40"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2028,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H33" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H34" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="39"/>
@@ -2099,7 +2099,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="21">
-        <v>0.25</v>
+        <v>0.95</v>
       </c>
       <c r="E9" s="59">
         <v>45007</v>
@@ -2180,7 +2180,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="59">
         <v>45009</v>
@@ -2259,7 +2259,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="21">
-        <v>0.01</v>
+        <v>0.95</v>
       </c>
       <c r="E11" s="59">
         <v>45011</v>
@@ -2335,7 +2335,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="21">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E12" s="59">
         <v>45005</v>
@@ -2487,7 +2487,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="60">
         <f>E10</f>
@@ -2568,7 +2568,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="26">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E15" s="60">
         <f>E14+2</f>
@@ -2646,7 +2646,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="26">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E16" s="60">
         <f>E14+1</f>
@@ -2724,7 +2724,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="26">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E17" s="60">
         <f>E12</f>
@@ -3074,7 +3074,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="61">
         <v>45008</v>
@@ -3153,7 +3153,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="31">
-        <v>0.35</v>
+        <v>0.95</v>
       </c>
       <c r="E23" s="61">
         <v>45009</v>
@@ -3220,7 +3220,7 @@
       <c r="BK23" s="39"/>
       <c r="BL23" s="39"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
       <c r="B24" s="75" t="s">
         <v>38</v>
@@ -3229,7 +3229,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="61">
         <v>45010</v>
@@ -3238,10 +3238,7 @@
         <v>45014</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="16">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
+      <c r="H24" s="16"/>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
       <c r="K24" s="39"/>
@@ -3299,29 +3296,29 @@
       <c r="BK24" s="39"/>
       <c r="BL24" s="39"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
       <c r="B25" s="75" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D25" s="31">
-        <v>2.5</v>
+        <v>0.15</v>
       </c>
       <c r="E25" s="61">
-        <f>F21+1</f>
-        <v>1</v>
+        <f>E12</f>
+        <v>45005</v>
       </c>
       <c r="F25" s="61">
-        <f t="shared" ref="F25:F33" si="4">E25+1</f>
-        <v>2</v>
+        <f>F12</f>
+        <v>45014</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
@@ -3389,20 +3386,20 @@
         <v>29</v>
       </c>
       <c r="D26" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="E26" s="61" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F26" s="61" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
+        <v>2.5</v>
+      </c>
+      <c r="E26" s="61">
+        <f>F21+1</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="61">
+        <f t="shared" ref="F26:F34" si="4">E26+1</f>
+        <v>2</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="16" t="e">
+      <c r="H26" s="16">
         <f t="shared" si="3"/>
-        <v>#REF!</v>
+        <v>2</v>
       </c>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
@@ -3470,20 +3467,20 @@
         <v>29</v>
       </c>
       <c r="D27" s="31">
-        <v>4.5</v>
-      </c>
-      <c r="E27" s="61">
-        <f>F22+1</f>
-        <v>45010</v>
-      </c>
-      <c r="F27" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="E27" s="61" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F27" s="61" t="e">
         <f t="shared" si="4"/>
-        <v>45011</v>
+        <v>#REF!</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="16">
+      <c r="H27" s="16" t="e">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>#REF!</v>
       </c>
       <c r="I27" s="39"/>
       <c r="J27" s="39"/>
@@ -3551,15 +3548,15 @@
         <v>29</v>
       </c>
       <c r="D28" s="31">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="E28" s="61">
-        <f t="shared" ref="E28:E33" si="5">F24+1</f>
-        <v>45015</v>
+        <f>F22+1</f>
+        <v>45010</v>
       </c>
       <c r="F28" s="61">
         <f t="shared" si="4"/>
-        <v>45016</v>
+        <v>45011</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16">
@@ -3632,15 +3629,15 @@
         <v>29</v>
       </c>
       <c r="D29" s="31">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="E29" s="61">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>F25+1</f>
+        <v>45015</v>
       </c>
       <c r="F29" s="61">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>45016</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16">
@@ -3713,20 +3710,20 @@
         <v>29</v>
       </c>
       <c r="D30" s="31">
-        <v>7.5</v>
-      </c>
-      <c r="E30" s="61" t="e">
-        <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F30" s="61" t="e">
+        <v>6.5</v>
+      </c>
+      <c r="E30" s="61">
+        <f t="shared" ref="E29:E34" si="5">F26+1</f>
+        <v>3</v>
+      </c>
+      <c r="F30" s="61">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
+        <v>4</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="16" t="e">
+      <c r="H30" s="16">
         <f t="shared" si="3"/>
-        <v>#REF!</v>
+        <v>2</v>
       </c>
       <c r="I30" s="39"/>
       <c r="J30" s="39"/>
@@ -3794,20 +3791,20 @@
         <v>29</v>
       </c>
       <c r="D31" s="31">
-        <v>8.5</v>
-      </c>
-      <c r="E31" s="61">
+        <v>7.5</v>
+      </c>
+      <c r="E31" s="61" t="e">
         <f t="shared" si="5"/>
-        <v>45012</v>
-      </c>
-      <c r="F31" s="61">
+        <v>#REF!</v>
+      </c>
+      <c r="F31" s="61" t="e">
         <f t="shared" si="4"/>
-        <v>45013</v>
+        <v>#REF!</v>
       </c>
       <c r="G31" s="16"/>
-      <c r="H31" s="16">
+      <c r="H31" s="16" t="e">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>#REF!</v>
       </c>
       <c r="I31" s="39"/>
       <c r="J31" s="39"/>
@@ -3875,15 +3872,15 @@
         <v>29</v>
       </c>
       <c r="D32" s="31">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="E32" s="61">
         <f t="shared" si="5"/>
-        <v>45017</v>
+        <v>45012</v>
       </c>
       <c r="F32" s="61">
         <f t="shared" si="4"/>
-        <v>45018</v>
+        <v>45013</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16">
@@ -3956,15 +3953,15 @@
         <v>29</v>
       </c>
       <c r="D33" s="31">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="E33" s="61">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>45017</v>
       </c>
       <c r="F33" s="61">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>45018</v>
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="16">
@@ -4028,15 +4025,30 @@
       <c r="BK33" s="39"/>
       <c r="BL33" s="39"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="31.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="53"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
+      <c r="B34" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="31">
+        <v>10.5</v>
+      </c>
+      <c r="E34" s="61">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F34" s="61">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
       <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="H34" s="16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="I34" s="39"/>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -4094,7 +4106,7 @@
       <c r="BK34" s="39"/>
       <c r="BL34" s="39"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="33.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="31.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="53"/>
       <c r="B35" s="76"/>
       <c r="C35" s="77"/>
@@ -4160,7 +4172,7 @@
       <c r="BK35" s="39"/>
       <c r="BL35" s="39"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="33.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="53"/>
       <c r="B36" s="76"/>
       <c r="C36" s="77"/>
@@ -4226,81 +4238,147 @@
       <c r="BK36" s="39"/>
       <c r="BL36" s="39"/>
     </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="54"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="41"/>
-      <c r="V37" s="41"/>
-      <c r="W37" s="41"/>
-      <c r="X37" s="41"/>
-      <c r="Y37" s="41"/>
-      <c r="Z37" s="41"/>
-      <c r="AA37" s="41"/>
-      <c r="AB37" s="41"/>
-      <c r="AC37" s="41"/>
-      <c r="AD37" s="41"/>
-      <c r="AE37" s="41"/>
-      <c r="AF37" s="41"/>
-      <c r="AG37" s="41"/>
-      <c r="AH37" s="41"/>
-      <c r="AI37" s="41"/>
-      <c r="AJ37" s="41"/>
-      <c r="AK37" s="41"/>
-      <c r="AL37" s="41"/>
-      <c r="AM37" s="41"/>
-      <c r="AN37" s="41"/>
-      <c r="AO37" s="41"/>
-      <c r="AP37" s="41"/>
-      <c r="AQ37" s="41"/>
-      <c r="AR37" s="41"/>
-      <c r="AS37" s="41"/>
-      <c r="AT37" s="41"/>
-      <c r="AU37" s="41"/>
-      <c r="AV37" s="41"/>
-      <c r="AW37" s="41"/>
-      <c r="AX37" s="41"/>
-      <c r="AY37" s="41"/>
-      <c r="AZ37" s="41"/>
-      <c r="BA37" s="41"/>
-      <c r="BB37" s="41"/>
-      <c r="BC37" s="41"/>
-      <c r="BD37" s="41"/>
-      <c r="BE37" s="41"/>
-      <c r="BF37" s="41"/>
-      <c r="BG37" s="41"/>
-      <c r="BH37" s="41"/>
-      <c r="BI37" s="41"/>
-      <c r="BJ37" s="41"/>
-      <c r="BK37" s="41"/>
-      <c r="BL37" s="41"/>
-    </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G38" s="6"/>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="53"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="39"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="39"/>
+      <c r="Z37" s="39"/>
+      <c r="AA37" s="39"/>
+      <c r="AB37" s="39"/>
+      <c r="AC37" s="39"/>
+      <c r="AD37" s="39"/>
+      <c r="AE37" s="39"/>
+      <c r="AF37" s="39"/>
+      <c r="AG37" s="39"/>
+      <c r="AH37" s="39"/>
+      <c r="AI37" s="39"/>
+      <c r="AJ37" s="39"/>
+      <c r="AK37" s="39"/>
+      <c r="AL37" s="39"/>
+      <c r="AM37" s="39"/>
+      <c r="AN37" s="39"/>
+      <c r="AO37" s="39"/>
+      <c r="AP37" s="39"/>
+      <c r="AQ37" s="39"/>
+      <c r="AR37" s="39"/>
+      <c r="AS37" s="39"/>
+      <c r="AT37" s="39"/>
+      <c r="AU37" s="39"/>
+      <c r="AV37" s="39"/>
+      <c r="AW37" s="39"/>
+      <c r="AX37" s="39"/>
+      <c r="AY37" s="39"/>
+      <c r="AZ37" s="39"/>
+      <c r="BA37" s="39"/>
+      <c r="BB37" s="39"/>
+      <c r="BC37" s="39"/>
+      <c r="BD37" s="39"/>
+      <c r="BE37" s="39"/>
+      <c r="BF37" s="39"/>
+      <c r="BG37" s="39"/>
+      <c r="BH37" s="39"/>
+      <c r="BI37" s="39"/>
+      <c r="BJ37" s="39"/>
+      <c r="BK37" s="39"/>
+      <c r="BL37" s="39"/>
+    </row>
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="54"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="41"/>
+      <c r="Z38" s="41"/>
+      <c r="AA38" s="41"/>
+      <c r="AB38" s="41"/>
+      <c r="AC38" s="41"/>
+      <c r="AD38" s="41"/>
+      <c r="AE38" s="41"/>
+      <c r="AF38" s="41"/>
+      <c r="AG38" s="41"/>
+      <c r="AH38" s="41"/>
+      <c r="AI38" s="41"/>
+      <c r="AJ38" s="41"/>
+      <c r="AK38" s="41"/>
+      <c r="AL38" s="41"/>
+      <c r="AM38" s="41"/>
+      <c r="AN38" s="41"/>
+      <c r="AO38" s="41"/>
+      <c r="AP38" s="41"/>
+      <c r="AQ38" s="41"/>
+      <c r="AR38" s="41"/>
+      <c r="AS38" s="41"/>
+      <c r="AT38" s="41"/>
+      <c r="AU38" s="41"/>
+      <c r="AV38" s="41"/>
+      <c r="AW38" s="41"/>
+      <c r="AX38" s="41"/>
+      <c r="AY38" s="41"/>
+      <c r="AZ38" s="41"/>
+      <c r="BA38" s="41"/>
+      <c r="BB38" s="41"/>
+      <c r="BC38" s="41"/>
+      <c r="BD38" s="41"/>
+      <c r="BE38" s="41"/>
+      <c r="BF38" s="41"/>
+      <c r="BG38" s="41"/>
+      <c r="BH38" s="41"/>
+      <c r="BI38" s="41"/>
+      <c r="BJ38" s="41"/>
+      <c r="BK38" s="41"/>
+      <c r="BL38" s="41"/>
     </row>
     <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="14"/>
-      <c r="F39" s="55"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="15"/>
+      <c r="C40" s="14"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4319,7 +4397,7 @@
     <mergeCell ref="L3:P3"/>
     <mergeCell ref="R3:V3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D37">
+  <conditionalFormatting sqref="D7:D38">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4333,12 +4411,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL37">
+  <conditionalFormatting sqref="I5:BL38">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL37">
+  <conditionalFormatting sqref="I7:BL38">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4373,7 +4451,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D37</xm:sqref>
+          <xm:sqref>D7:D38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>